<commit_message>
update Excel file version
</commit_message>
<xml_diff>
--- a/wiki-files/RE2020_ONV_Outil_Saisie_Manuelle_v1.xlsx
+++ b/wiki-files/RE2020_ONV_Outil_Saisie_Manuelle_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16428" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" tabRatio="679" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mode d'emploi" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
   <si>
     <t>Version du schéma de fichier :</t>
   </si>
@@ -964,6 +964,9 @@
       <t xml:space="preserve"> "débit de base".</t>
     </r>
   </si>
+  <si>
+    <t>1.2</t>
+  </si>
 </sst>
 </file>
 
@@ -1602,6 +1605,42 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1640,42 +1679,6 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1684,6 +1687,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1711,8 +1716,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1981,21 +1984,21 @@
     </row>
     <row r="7" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:13" s="35" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
     </row>
     <row r="9" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2069,21 +2072,21 @@
       <c r="M13" s="45"/>
     </row>
     <row r="14" spans="1:13" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="71"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="83"/>
     </row>
     <row r="15" spans="1:13" s="35" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
@@ -2102,139 +2105,139 @@
     </row>
     <row r="16" spans="1:13" s="35" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="73"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="85"/>
     </row>
     <row r="17" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="75"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="87"/>
     </row>
     <row r="18" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="77"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="89"/>
     </row>
     <row r="19" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="77"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="89"/>
     </row>
     <row r="20" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="77"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="89"/>
     </row>
     <row r="21" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46"/>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="77"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="89"/>
     </row>
     <row r="22" spans="1:21" s="35" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="66"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="78"/>
     </row>
     <row r="23" spans="1:21" s="35" customFormat="1" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="48"/>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="68"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="80"/>
     </row>
     <row r="24" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -2258,40 +2261,40 @@
       <c r="A26" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="86"/>
-      <c r="M26" s="86"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
       <c r="N26" s="57"/>
     </row>
     <row r="27" spans="1:21" ht="49.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="88"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="74"/>
       <c r="N27" s="52"/>
       <c r="O27" s="52"/>
       <c r="P27" s="52"/>
@@ -2302,23 +2305,23 @@
       <c r="U27" s="52"/>
     </row>
     <row r="28" spans="1:21" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="85"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="71"/>
       <c r="N28" s="54"/>
       <c r="O28" s="55"/>
       <c r="P28" s="55"/>
@@ -2329,39 +2332,39 @@
       <c r="U28" s="56"/>
     </row>
     <row r="29" spans="1:21" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
-      <c r="B29" s="89" t="s">
+      <c r="A29" s="68"/>
+      <c r="B29" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="84"/>
-      <c r="M29" s="84"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
       <c r="N29" s="59"/>
     </row>
     <row r="30" spans="1:21" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="78" t="s">
+      <c r="A30" s="69"/>
+      <c r="B30" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="80"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="66"/>
       <c r="N30" s="59"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -2381,12 +2384,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B29:M29"/>
     <mergeCell ref="A8:M8"/>
     <mergeCell ref="B22:M22"/>
     <mergeCell ref="B23:M23"/>
@@ -2397,6 +2394,12 @@
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B20:M20"/>
     <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B29:M29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2411,7 +2414,7 @@
   <dimension ref="A1:H1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2436,12 +2439,12 @@
       <c r="A2" s="1"/>
       <c r="B2" s="32"/>
       <c r="C2" s="1"/>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="108"/>
-      <c r="G2" s="2">
-        <v>1</v>
+      <c r="F2" s="95"/>
+      <c r="G2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -2456,15 +2459,15 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="96" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="91"/>
       <c r="E4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="93"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2689,7 +2692,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="91"/>
@@ -5078,39 +5081,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
       <c r="N1" s="91"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="20" t="s">
         <v>23</v>
       </c>
@@ -11013,28 +11016,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="104" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="102" t="s">
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="106"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="25" t="s">
         <v>86</v>
       </c>

</xml_diff>